<commit_message>
Each character is now printable. Dropped powers that caused problems during data fetch from compendium. This means I don't always have optimal powers anymore. May Hand-craft the problem powers.
</commit_message>
<xml_diff>
--- a/4e/AoE hammer delve/party makeup.xlsx
+++ b/4e/AoE hammer delve/party makeup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="18270" windowHeight="7900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="7900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Count</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Dragonborn</t>
   </si>
   <si>
-    <t>Use rod to go rainbow: everything is radiant + thuner in paragon</t>
-  </si>
-  <si>
     <t>Long</t>
   </si>
   <si>
@@ -99,6 +96,15 @@
   </si>
   <si>
     <t>Artificer</t>
+  </si>
+  <si>
+    <t>Use rod to go rainbow: everything is radiant + thunder in paragon</t>
+  </si>
+  <si>
+    <t>Invoker</t>
+  </si>
+  <si>
+    <t>Shardmind</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,64 +473,75 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>